<commit_message>
Added unique "refreshable_vins" for each product. Corrected some update files Corrected DB update and cleanup queries
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New7VIN_CA_SELECT.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New7VIN_CA_SELECT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Desktop\SUITE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,8 +23,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Petrenko, Viktor (C)</author>
+  </authors>
+  <commentList>
+    <comment ref="AA6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Petrenko, Viktor (C):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+User for MSRP PAS-730</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="81">
   <si>
     <t>VIN</t>
   </si>
@@ -225,13 +259,55 @@
   </si>
   <si>
     <t>GGGNK2CC&amp;F</t>
+  </si>
+  <si>
+    <t>7MSRP15H&amp;V</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN</t>
+  </si>
+  <si>
+    <t>GOLF</t>
+  </si>
+  <si>
+    <t>HATCHBACK 4 DOOR</t>
+  </si>
+  <si>
+    <t>8L V12</t>
+  </si>
+  <si>
+    <t>4WD</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>BBBKN3DD&amp;E</t>
+  </si>
+  <si>
+    <t>MAKEPAS2713ENDOR</t>
+  </si>
+  <si>
+    <t>MODELPAS2713ENDOR</t>
+  </si>
+  <si>
+    <t>SERIESPAS2713ENDOR</t>
+  </si>
+  <si>
+    <t>BODYTYPEPAS2713ENDOR</t>
+  </si>
+  <si>
+    <t>BODYSTYLEPAS2713ENDOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +327,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -566,11 +655,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,8 +1258,238 @@
         <v>50</v>
       </c>
     </row>
+    <row r="6" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="3">
+        <v>88888</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="3">
+        <v>12</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>214</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="S6" s="3">
+        <v>4</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" s="3">
+        <v>2</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>33</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>43</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>20000101</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7">
+        <v>2018</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7">
+        <v>88888</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" t="s">
+        <v>71</v>
+      </c>
+      <c r="O7">
+        <v>12</v>
+      </c>
+      <c r="P7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7">
+        <v>214</v>
+      </c>
+      <c r="R7" t="s">
+        <v>72</v>
+      </c>
+      <c r="S7">
+        <v>4</v>
+      </c>
+      <c r="T7" t="s">
+        <v>33</v>
+      </c>
+      <c r="U7" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7">
+        <v>2</v>
+      </c>
+      <c r="W7" t="s">
+        <v>35</v>
+      </c>
+      <c r="X7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA7">
+        <v>33</v>
+      </c>
+      <c r="AB7">
+        <v>43</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI7">
+        <v>20000101</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>